<commit_message>
docker containers 19/03/2025 excel sheet
</commit_message>
<xml_diff>
--- a/docker_container_details.xlsx
+++ b/docker_container_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4638273d6294cea6/Desktop/internship/puropale_document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{646B6136-7BC2-498C-B4CA-6847101C42FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{646B6136-7BC2-498C-B4CA-6847101C42FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F247BFB-4F8C-4DC2-B559-350FCEC53FCB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{663A684B-38D7-4984-949B-B822EA6C693F}"/>
+    <workbookView xWindow="3348" yWindow="3348" windowWidth="10332" windowHeight="6000" xr2:uid="{663A684B-38D7-4984-949B-B822EA6C693F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Sl.No</t>
   </si>
@@ -102,6 +91,9 @@
   </si>
   <si>
     <t>83d938198316</t>
+  </si>
+  <si>
+    <t>8.0.52</t>
   </si>
 </sst>
 </file>
@@ -456,7 +448,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +535,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>